<commit_message>
UPDATED: jsons & excels
</commit_message>
<xml_diff>
--- a/data/common/excel/public_category_manual.xlsx
+++ b/data/common/excel/public_category_manual.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OPT Design\PycharmProjects\optima-scrapper\data\common\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F8811B9-65E2-4507-B0E3-708723E48838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{595D8988-CE78-4813-8574-9B2DC2F01F69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{98414BF8-B91D-4538-8B60-2AD3F6A6ADCC}"/>
+    <workbookView xWindow="29775" yWindow="1305" windowWidth="18930" windowHeight="14235" xr2:uid="{98414BF8-B91D-4538-8B60-2AD3F6A6ADCC}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="37">
   <si>
     <t>SKU</t>
   </si>
@@ -112,6 +112,30 @@
   </si>
   <si>
     <t>FAROLAS LED</t>
+  </si>
+  <si>
+    <t>BOMBILLAS LED SMART</t>
+  </si>
+  <si>
+    <t>212756 </t>
+  </si>
+  <si>
+    <t>3001 </t>
+  </si>
+  <si>
+    <t>2999 </t>
+  </si>
+  <si>
+    <t>212754 </t>
+  </si>
+  <si>
+    <t>2755 </t>
+  </si>
+  <si>
+    <t>2751 </t>
+  </si>
+  <si>
+    <t>APARATOS SMART</t>
   </si>
 </sst>
 </file>
@@ -727,10 +751,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BF40A98-2910-49B0-BB76-BAF76F0B7575}">
-  <dimension ref="A1:C109"/>
+  <dimension ref="A1:C117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C105" sqref="C105"/>
+    <sheetView tabSelected="1" topLeftCell="A84" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B100" sqref="B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1703,6 +1727,70 @@
         <v>3903</v>
       </c>
     </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C110" s="5">
+        <v>2755</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C111" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C112" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C113" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C114" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C115" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C116" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="C117" s="5">
+        <v>8445</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>